<commit_message>
updated queries with responses for booleans search
</commit_message>
<xml_diff>
--- a/Project1_queries.xlsx
+++ b/Project1_queries.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikee\Desktop\School\Fall_2022\COS 470\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikee\Desktop\School\Fall_2022\COS 470\project\IRCourse-TiffanyHoeung-MikeBelley\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53072309-1B13-4E7E-A154-4DA1485A6178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713BB1CC-1B94-4536-BAFB-1271AE04ED02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1BFBBF9-F489-484B-B5E6-DD464C47654C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{D1BFBBF9-F489-484B-B5E6-DD464C47654C}"/>
   </bookViews>
   <sheets>
     <sheet name="All queries" sheetId="1" r:id="rId1"/>
     <sheet name="Inverted Index" sheetId="2" r:id="rId2"/>
     <sheet name="Boolean" sheetId="3" r:id="rId3"/>
+    <sheet name="Boolean Scores" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="42">
   <si>
     <t>Question</t>
   </si>
@@ -161,6 +162,9 @@
   </si>
   <si>
     <t>Information Need</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -190,10 +194,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -202,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -215,6 +228,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4A1410-AA0E-4A6E-A514-B6E6C2A54DF2}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -743,12 +760,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B1" t="s">
@@ -759,7 +776,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -767,19 +784,19 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -787,19 +804,19 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -807,19 +824,19 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -827,19 +844,19 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -847,19 +864,19 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -867,19 +884,19 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -887,7 +904,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
@@ -908,131 +925,128 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C11A7FE6-FE9E-4387-A006-7B68B23530B2}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1040,19 +1054,19 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1060,7 +1074,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1077,4 +1091,670 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3210BD09-D174-4B50-9A12-80B486FEBE32}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="5" max="5" width="9.140625" style="5"/>
+    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="9" max="9" width="9.140625" style="5"/>
+    <col min="11" max="11" width="9.140625" style="5"/>
+    <col min="13" max="13" width="9.140625" style="5"/>
+    <col min="15" max="15" width="9.140625" style="5"/>
+    <col min="17" max="17" width="9.140625" style="5"/>
+    <col min="19" max="19" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1073</v>
+      </c>
+      <c r="D2">
+        <v>1691</v>
+      </c>
+      <c r="F2">
+        <v>1693</v>
+      </c>
+      <c r="H2">
+        <v>1701</v>
+      </c>
+      <c r="J2">
+        <v>2135</v>
+      </c>
+      <c r="L2">
+        <v>2291</v>
+      </c>
+      <c r="N2">
+        <v>2381</v>
+      </c>
+      <c r="P2">
+        <v>3613</v>
+      </c>
+      <c r="R2">
+        <v>5541</v>
+      </c>
+      <c r="T2">
+        <v>8524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>151499</v>
+      </c>
+      <c r="D3">
+        <v>188057</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>525</v>
+      </c>
+      <c r="D5">
+        <v>1572</v>
+      </c>
+      <c r="F5">
+        <v>1709</v>
+      </c>
+      <c r="H5">
+        <v>2680</v>
+      </c>
+      <c r="J5">
+        <v>3039</v>
+      </c>
+      <c r="L5">
+        <v>3310</v>
+      </c>
+      <c r="N5">
+        <v>3434</v>
+      </c>
+      <c r="P5">
+        <v>3435</v>
+      </c>
+      <c r="R5">
+        <v>3961</v>
+      </c>
+      <c r="T5">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>47326</v>
+      </c>
+      <c r="D6">
+        <v>50468</v>
+      </c>
+      <c r="F6">
+        <v>55793</v>
+      </c>
+      <c r="H6">
+        <v>59250</v>
+      </c>
+      <c r="J6">
+        <v>70567</v>
+      </c>
+      <c r="L6">
+        <v>71546</v>
+      </c>
+      <c r="N6">
+        <v>95945</v>
+      </c>
+      <c r="P6">
+        <v>129984</v>
+      </c>
+      <c r="R6">
+        <v>134056</v>
+      </c>
+      <c r="T6">
+        <v>140629</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>143</v>
+      </c>
+      <c r="D8">
+        <v>255</v>
+      </c>
+      <c r="F8">
+        <v>268</v>
+      </c>
+      <c r="H8">
+        <v>369</v>
+      </c>
+      <c r="J8">
+        <v>372</v>
+      </c>
+      <c r="L8">
+        <v>374</v>
+      </c>
+      <c r="N8">
+        <v>376</v>
+      </c>
+      <c r="P8">
+        <v>383</v>
+      </c>
+      <c r="R8">
+        <v>394</v>
+      </c>
+      <c r="T8">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>6184</v>
+      </c>
+      <c r="D9">
+        <v>21888</v>
+      </c>
+      <c r="F9">
+        <v>35344</v>
+      </c>
+      <c r="H9">
+        <v>36423</v>
+      </c>
+      <c r="J9">
+        <v>37475</v>
+      </c>
+      <c r="L9">
+        <v>38341</v>
+      </c>
+      <c r="N9">
+        <v>42179</v>
+      </c>
+      <c r="P9">
+        <v>45480</v>
+      </c>
+      <c r="R9">
+        <v>48251</v>
+      </c>
+      <c r="T9">
+        <v>53429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>71043</v>
+      </c>
+      <c r="D10">
+        <v>71593</v>
+      </c>
+      <c r="F10">
+        <v>114180</v>
+      </c>
+      <c r="H10">
+        <v>123457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>88</v>
+      </c>
+      <c r="F11">
+        <v>93</v>
+      </c>
+      <c r="H11">
+        <v>159</v>
+      </c>
+      <c r="J11">
+        <v>207</v>
+      </c>
+      <c r="L11">
+        <v>229</v>
+      </c>
+      <c r="N11">
+        <v>283</v>
+      </c>
+      <c r="P11">
+        <v>481</v>
+      </c>
+      <c r="R11">
+        <v>535</v>
+      </c>
+      <c r="T11">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>71</v>
+      </c>
+      <c r="D12">
+        <v>88</v>
+      </c>
+      <c r="F12">
+        <v>93</v>
+      </c>
+      <c r="H12">
+        <v>207</v>
+      </c>
+      <c r="J12">
+        <v>229</v>
+      </c>
+      <c r="L12">
+        <v>283</v>
+      </c>
+      <c r="N12">
+        <v>595</v>
+      </c>
+      <c r="P12">
+        <v>799</v>
+      </c>
+      <c r="R12">
+        <v>1473</v>
+      </c>
+      <c r="T12">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>283</v>
+      </c>
+      <c r="D13">
+        <v>13827</v>
+      </c>
+      <c r="F13">
+        <v>20166</v>
+      </c>
+      <c r="H13">
+        <v>24934</v>
+      </c>
+      <c r="J13">
+        <v>29818</v>
+      </c>
+      <c r="L13">
+        <v>30766</v>
+      </c>
+      <c r="N13">
+        <v>31267</v>
+      </c>
+      <c r="P13">
+        <v>34984</v>
+      </c>
+      <c r="R13">
+        <v>35029</v>
+      </c>
+      <c r="T13">
+        <v>36656</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1845</v>
+      </c>
+      <c r="D14">
+        <v>16664</v>
+      </c>
+      <c r="F14">
+        <v>19217</v>
+      </c>
+      <c r="H14">
+        <v>24811</v>
+      </c>
+      <c r="J14">
+        <v>37076</v>
+      </c>
+      <c r="L14">
+        <v>59770</v>
+      </c>
+      <c r="N14">
+        <v>73590</v>
+      </c>
+      <c r="P14">
+        <v>79801</v>
+      </c>
+      <c r="R14">
+        <v>92079</v>
+      </c>
+      <c r="T14">
+        <v>102305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>1845</v>
+      </c>
+      <c r="D15">
+        <v>16664</v>
+      </c>
+      <c r="F15">
+        <v>59770</v>
+      </c>
+      <c r="H15">
+        <v>73590</v>
+      </c>
+      <c r="J15">
+        <v>92079</v>
+      </c>
+      <c r="L15">
+        <v>104760</v>
+      </c>
+      <c r="N15">
+        <v>114740</v>
+      </c>
+      <c r="P15">
+        <v>125692</v>
+      </c>
+      <c r="R15">
+        <v>150990</v>
+      </c>
+      <c r="T15">
+        <v>161363</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>16664</v>
+      </c>
+      <c r="D16">
+        <v>150990</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>1165</v>
+      </c>
+      <c r="D17">
+        <v>2150</v>
+      </c>
+      <c r="F17">
+        <v>2495</v>
+      </c>
+      <c r="H17">
+        <v>4540</v>
+      </c>
+      <c r="J17">
+        <v>5034</v>
+      </c>
+      <c r="L17">
+        <v>5220</v>
+      </c>
+      <c r="N17">
+        <v>5229</v>
+      </c>
+      <c r="P17">
+        <v>5779</v>
+      </c>
+      <c r="R17">
+        <v>6011</v>
+      </c>
+      <c r="T17">
+        <v>6221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>2150</v>
+      </c>
+      <c r="D18">
+        <v>2495</v>
+      </c>
+      <c r="F18">
+        <v>7486</v>
+      </c>
+      <c r="H18">
+        <v>7919</v>
+      </c>
+      <c r="J18">
+        <v>8208</v>
+      </c>
+      <c r="L18">
+        <v>8656</v>
+      </c>
+      <c r="N18">
+        <v>10442</v>
+      </c>
+      <c r="P18">
+        <v>11614</v>
+      </c>
+      <c r="R18">
+        <v>12168</v>
+      </c>
+      <c r="T18">
+        <v>12460</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>2150</v>
+      </c>
+      <c r="D19">
+        <v>7486</v>
+      </c>
+      <c r="F19">
+        <v>12168</v>
+      </c>
+      <c r="H19">
+        <v>12604</v>
+      </c>
+      <c r="J19">
+        <v>14184</v>
+      </c>
+      <c r="L19">
+        <v>16143</v>
+      </c>
+      <c r="N19">
+        <v>19558</v>
+      </c>
+      <c r="P19">
+        <v>19946</v>
+      </c>
+      <c r="R19">
+        <v>22033</v>
+      </c>
+      <c r="T19">
+        <v>22442</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <v>60</v>
+      </c>
+      <c r="F20">
+        <v>330</v>
+      </c>
+      <c r="H20">
+        <v>338</v>
+      </c>
+      <c r="J20">
+        <v>902</v>
+      </c>
+      <c r="L20">
+        <v>1776</v>
+      </c>
+      <c r="N20">
+        <v>1861</v>
+      </c>
+      <c r="P20">
+        <v>1862</v>
+      </c>
+      <c r="R20">
+        <v>2638</v>
+      </c>
+      <c r="T20">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>338</v>
+      </c>
+      <c r="D21">
+        <v>3646</v>
+      </c>
+      <c r="F21">
+        <v>5112</v>
+      </c>
+      <c r="H21">
+        <v>5262</v>
+      </c>
+      <c r="J21">
+        <v>5472</v>
+      </c>
+      <c r="L21">
+        <v>5573</v>
+      </c>
+      <c r="N21">
+        <v>5809</v>
+      </c>
+      <c r="P21">
+        <v>6112</v>
+      </c>
+      <c r="R21">
+        <v>6544</v>
+      </c>
+      <c r="T21">
+        <v>6557</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>